<commit_message>
metadata title change from volume to album
</commit_message>
<xml_diff>
--- a/clo-angular/src/assets/albums/fullsize/album_04/Volume4.xlsx
+++ b/clo-angular/src/assets/albums/fullsize/album_04/Volume4.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stella/clo3/clo-angular/src/assets/albums/fullsize/album_04/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA5A6FB-E060-194B-A5EB-75D8B66ABF46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="109">
   <si>
     <t>title_of_work</t>
   </si>
@@ -67,9 +76,6 @@
     <t>Page 1</t>
   </si>
   <si>
-    <t>Carlyle Photograph Albums, Volume 4, Page 1</t>
-  </si>
-  <si>
     <t>Three photographs; portraits in oval and rectangle frames. Inscriptions read, "Wm Penn"; "Qn Elizabeth" [QEI]; and "Prince Albert."</t>
   </si>
   <si>
@@ -109,27 +115,18 @@
     <t>Page 2</t>
   </si>
   <si>
-    <t>Carlyle Photograph Albums, Volume 4, Page 2</t>
-  </si>
-  <si>
     <t>Four photographs, with inscriptions: "Very bad Picture of R. Waldo Emerson (Concord, Mass)"; "Theodore Parker (Boston)"; "Cushman"; and the fourth, autographed: "Gius. Mazzini."</t>
   </si>
   <si>
     <t>Page 3</t>
   </si>
   <si>
-    <t>Carlyle Photograph Albums, Volume 4, Page 3</t>
-  </si>
-  <si>
     <t>Four photographs, inscribed: "Dr Barnes" [the elder]; "Fredc Pollock"; "Revd Rector Blunt (1864)"; and "Miss Royston."</t>
   </si>
   <si>
     <t>Page 4</t>
   </si>
   <si>
-    <t>Carlyle Photograph Albums, Volume 4, Page 4</t>
-  </si>
-  <si>
     <t>Four photographs, inscribed: "Madme Otthennin de &amp;c";  "Madlle Otthennin de St. Julien"; "T. Woolner (1864)"; and "Paris, October 1862" "(Browning jun?)."</t>
   </si>
   <si>
@@ -142,72 +139,48 @@
     <t>Page 5</t>
   </si>
   <si>
-    <t>Carlyle Photograph Albums, Volume 4, Page 5</t>
-  </si>
-  <si>
     <t>Four photographs, inscribed: "Mrs. Symons (once Miss Barnes)"; "Dr Garth Wilkinson"; "John Bright M.P."; and "Miss Royston."</t>
   </si>
   <si>
     <t>Page 6</t>
   </si>
   <si>
-    <t>Carlyle Photograph Albums, Volume 4, Page 6</t>
-  </si>
-  <si>
     <t xml:space="preserve">Four photographs, inscribed: "Miss W. Wynn"; unidentified woman standing, from the back; not in Thomas Carlyle's hand: "Mrs Russell's maid, Mary" and an unidentified male figure, standing. </t>
   </si>
   <si>
     <t>Page 7</t>
   </si>
   <si>
-    <t>Carlyle Photograph Albums, Volume 4, Page 7</t>
-  </si>
-  <si>
     <t xml:space="preserve">Three images: photograph of an engraving inscribed "Kaalback's Frederick the Great (not the least like) / 1864"; a photograph portrait of an unidentified woman, and a caricature, drawn by Elizabeth Paulet in 1844 titled "Notre Dame de Chelsea." </t>
   </si>
   <si>
     <t>Page 8</t>
   </si>
   <si>
-    <t>Carlyle Photograph Albums, Volume 4, Page 8</t>
-  </si>
-  <si>
     <t xml:space="preserve">Four photographs, inscribed "Painter Hunt?"; "My Jane: --Like"; "Plattnauer"; and a photograph of an unidentified couple and two young girls. </t>
   </si>
   <si>
     <t>Page 9</t>
   </si>
   <si>
-    <t>Carlyle Photograph Albums, Volume 4, Page 9</t>
-  </si>
-  <si>
     <t>Three images: a churchyard cemetery in closeup, inscribed "Wordsworth's Grave (Grasmere, 1863)"; an oval portrait of "Oliver Cromwell's Mother" and a churchyard from a distance, inscribed: "St Mary Ottery, Devon" [near the birthplace of Coleridge].</t>
   </si>
   <si>
     <t>Page 10</t>
   </si>
   <si>
-    <t>Carlyle Photograph Albums, Volume 4, Page 10</t>
-  </si>
-  <si>
     <t>Four photographs of buildings, inscribed: "Haugh (Haddington); "Co[mmercia]l Bank (Haddington)"; "Haddington Church" and "Haddington."</t>
   </si>
   <si>
     <t>Page 11</t>
   </si>
   <si>
-    <t>Carlyle Photograph Albums, Volume 4, Page 11</t>
-  </si>
-  <si>
     <t>Four photographs, inscribed: "Fredc Foxton"; "me (in 1863)"; "'Charlotte' (Servant here)" and "My Jane:--not good."</t>
   </si>
   <si>
     <t>Page 12</t>
   </si>
   <si>
-    <t>Carlyle Photograph Albums, Volume 4, Page 12</t>
-  </si>
-  <si>
     <t xml:space="preserve">Four images: a pen &amp; ink drawing of a large rock formation, perhaps on a beach, with two figures in the foreground, possibly drawn by Ruskin; a photograph of a seated "Miss Constance E. Kent" [murderer, by axe, of her young step-brother]; a photograph of the west front of the cathedral in Exeter; and a photograph of Dr. E.W. Pritchard , inscribed "wife-poisoner" by Carlyle. </t>
   </si>
   <si>
@@ -220,9 +193,6 @@
     <t>Page 13</t>
   </si>
   <si>
-    <t>Carlyle Photograph Albums, Volume 4, Page 13</t>
-  </si>
-  <si>
     <t xml:space="preserve">Four photographs of men, inscribed: "Germn Tailor / Franz Müller," with umlaut added by Thomas Carlyle as well as "1864" and "(murderer!)" "in a railway"; a photograph of a man inscribed "Parsons, Painter, Photogr &amp;c"; a small oval photograph of a man inscribed "C.G. Duffy" and a photograph of a man, standing in left profile, inscribed: "Major Venturi." </t>
   </si>
   <si>
@@ -232,63 +202,42 @@
     <t>Page 14</t>
   </si>
   <si>
-    <t>Carlyle Photograph Albums, Volume 4, Page 14</t>
-  </si>
-  <si>
     <t xml:space="preserve">Five photographs: in a small oval, an elderly man with white hair, bushy eyebrows, and beard, bearing a faint resemblance to Thomas Carlyle in old age; and photographs of women, inscribed "Miss Hogarth, Dicken's sister-in-law"; "Miss Dickens?"; Jane Welsh Carlyle, faint, in oval inscribed "from a bad picture of her" and a photograph of a seated man, inscribed "Dr Barnes." </t>
   </si>
   <si>
     <t>Page 15</t>
   </si>
   <si>
-    <t>Carlyle Photograph Albums, Volume 4, Page 15</t>
-  </si>
-  <si>
     <t>Four photographs of men, inscribed: "Abraham Lincoln"; the word "and" between the photos, then, "J.W. Booth" "his assassin"; "Duffy agn" [Elliott &amp; Fry studio photo] and "Giu. Mazzini."</t>
   </si>
   <si>
     <t>Page 16</t>
   </si>
   <si>
-    <t>Carlyle Photograph Albums, Volume 4, Page 16</t>
-  </si>
-  <si>
     <t>Four photographs, all of Jane Welsh Carlyle, all seated; two vignettes, one inscribed "from a picture", the other "do of Her: all bad,--this the worst."</t>
   </si>
   <si>
     <t>Page 17</t>
   </si>
   <si>
-    <t>Carlyle Photograph Albums, Volume 4, Page 17</t>
-  </si>
-  <si>
     <t>Four photographs: at top, vignettes of two Confederate officers,  inscribed: "Thomson, a Virgin[ia]n : writer, ex-Volunteer, &amp;c" and "another Virgin[ia]n, ex- &amp;c"; a photograph of a woman in right profile, inscribed: "Madame Venturi (born Ashhurst)" and a photograph of a couple, inscribed: "Venturi &amp; wife."</t>
   </si>
   <si>
     <t>Page 18</t>
   </si>
   <si>
-    <t>Carlyle Photograph Albums, Volume 4, Page 18</t>
-  </si>
-  <si>
     <t>Four photographs, inscribed: "Macmillan, Publisher"; an unidentified woman, seated; "a Canad[ia]n Nephew" and "do Tom?"</t>
   </si>
   <si>
     <t>Page 19</t>
   </si>
   <si>
-    <t>Carlyle Photograph Albums, Volume 4, Page 19</t>
-  </si>
-  <si>
     <t>Seven photographs: a seated woman, inscribed: "G.E. Jewsbury"; four small ovals of Jane Welsh Carlyle on a single card, inscribed "(all sadly unlike!)"; two photographs of a standing women inscribed "Aunt Grace" and 'Mrs Warren,' our servant."</t>
   </si>
   <si>
     <t>Page 20</t>
   </si>
   <si>
-    <t>Carlyle Photograph Albums, Volume 4, Page 20</t>
-  </si>
-  <si>
     <t>Four images, all prints: a reproduction of a print of Jesus with the first apostles in their boat with their nets; cartoon of Thomas Carlyle crushed under the weight of Frederick; an image of the Apotheosis of Washington and Lincoln; and Thomas Carlyle with shovel and pail with printed inscription, "writing 'finis' to Friedrich, altogether...off to Scarborough in this summer weather."</t>
   </si>
   <si>
@@ -298,68 +247,115 @@
     <t>Page 21</t>
   </si>
   <si>
-    <t>Carlyle Photograph Albums, Volume 4, Page 21</t>
-  </si>
-  <si>
     <t xml:space="preserve">Four photographs, two portraits and two photographs of busts, inscribed :"Miss Hetty Reichenbach"; a bust of "our Coll Davidson (Haddn)?"; "Bust of Ld Ashburton (unlike)"; and "Dr. Barnes the younger." </t>
   </si>
   <si>
     <t>Page 22</t>
   </si>
   <si>
-    <t>Carlyle Photograph Albums, Volume 4, Page 22</t>
-  </si>
-  <si>
     <t>A large, vertically oriented photograph of a building and trees, inscribed: "Auchtertool (Fife)."</t>
   </si>
   <si>
     <t>Page 23</t>
   </si>
   <si>
-    <t>Carlyle Photograph Albums, Volume 4, Page 23</t>
-  </si>
-  <si>
     <t>Four photographs: three of John Ruskin one of Geraldine Jewsbury.</t>
   </si>
   <si>
     <t>Page 24</t>
   </si>
   <si>
-    <t>Carlyle Photograph Albums, Volume 4, Page 24</t>
-  </si>
-  <si>
     <t xml:space="preserve">Four photographs: inscribed "Dr Carlyle my Brr" and "Mrs Sterling (T. Erskine's sister)"; followed by two photographs of John Ruskin. </t>
   </si>
   <si>
     <t>Page 25</t>
   </si>
   <si>
-    <t>Carlyle Photograph Albums, Volume 4, Page 25</t>
-  </si>
-  <si>
     <t>Photograph of Jane Welsh Carlyle, inscribed by Robert Scott Tait: "28th July 1854"; also inscribed by Thomas Carlyle: "(by Tait): some considble likeness."</t>
+  </si>
+  <si>
+    <t>Carlyle Photograph Albums, Album 4, Page 1</t>
+  </si>
+  <si>
+    <t>Carlyle Photograph Albums, Album 4, Page 2</t>
+  </si>
+  <si>
+    <t>Carlyle Photograph Albums, Album 4, Page 3</t>
+  </si>
+  <si>
+    <t>Carlyle Photograph Albums, Album 4, Page 4</t>
+  </si>
+  <si>
+    <t>Carlyle Photograph Albums, Album 4, Page 5</t>
+  </si>
+  <si>
+    <t>Carlyle Photograph Albums, Album 4, Page 6</t>
+  </si>
+  <si>
+    <t>Carlyle Photograph Albums, Album 4, Page 7</t>
+  </si>
+  <si>
+    <t>Carlyle Photograph Albums, Album 4, Page 8</t>
+  </si>
+  <si>
+    <t>Carlyle Photograph Albums, Album 4, Page 9</t>
+  </si>
+  <si>
+    <t>Carlyle Photograph Albums, Album 4, Page 10</t>
+  </si>
+  <si>
+    <t>Carlyle Photograph Albums, Album 4, Page 11</t>
+  </si>
+  <si>
+    <t>Carlyle Photograph Albums, Album 4, Page 12</t>
+  </si>
+  <si>
+    <t>Carlyle Photograph Albums, Album 4, Page 13</t>
+  </si>
+  <si>
+    <t>Carlyle Photograph Albums, Album 4, Page 14</t>
+  </si>
+  <si>
+    <t>Carlyle Photograph Albums, Album 4, Page 15</t>
+  </si>
+  <si>
+    <t>Carlyle Photograph Albums, Album 4, Page 16</t>
+  </si>
+  <si>
+    <t>Carlyle Photograph Albums, Album 4, Page 17</t>
+  </si>
+  <si>
+    <t>Carlyle Photograph Albums, Album 4, Page 18</t>
+  </si>
+  <si>
+    <t>Carlyle Photograph Albums, Album 4, Page 19</t>
+  </si>
+  <si>
+    <t>Carlyle Photograph Albums, Album 4, Page 20</t>
+  </si>
+  <si>
+    <t>Carlyle Photograph Albums, Album 4, Page 21</t>
+  </si>
+  <si>
+    <t>Carlyle Photograph Albums, Album 4, Page 22</t>
+  </si>
+  <si>
+    <t>Carlyle Photograph Albums, Album 4, Page 23</t>
+  </si>
+  <si>
+    <t>Carlyle Photograph Albums, Album 4, Page 24</t>
+  </si>
+  <si>
+    <t>Carlyle Photograph Albums, Album 4, Page 25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -455,41 +451,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,25 +474,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffececec"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFECECEC"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -718,7 +754,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -737,7 +773,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -767,7 +803,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -793,7 +829,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -819,7 +855,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -845,7 +881,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -871,7 +907,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -897,7 +933,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -923,7 +959,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -949,7 +985,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -975,7 +1011,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -988,9 +1024,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1007,7 +1049,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1026,7 +1068,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1052,7 +1094,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1078,7 +1120,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1104,7 +1146,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1130,7 +1172,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1156,7 +1198,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1182,7 +1224,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1208,7 +1250,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1234,7 +1276,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1260,7 +1302,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1273,9 +1315,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1289,7 +1337,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1308,7 +1356,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1338,7 +1386,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1364,7 +1412,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1390,7 +1438,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1416,7 +1464,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1442,7 +1490,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1468,7 +1516,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1494,7 +1542,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1520,7 +1568,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1546,7 +1594,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1559,1437 +1607,1446 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.25" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" style="1" customWidth="1"/>
-    <col min="2" max="2" width="2.67188" style="1" customWidth="1"/>
+    <col min="2" max="2" width="2.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="44.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="77" style="1" customWidth="1"/>
-    <col min="5" max="21" width="8.85156" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="5" max="22" width="8.83203125" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.15" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:21" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="3">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="4">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="5">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="6">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="6">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s" s="6">
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s" s="6">
+      <c r="H1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s" s="6">
+      <c r="I1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s" s="6">
+      <c r="J1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s" s="6">
+      <c r="K1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L1" t="s" s="6">
+      <c r="L1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="M1" t="s" s="6">
+      <c r="M1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N1" t="s" s="6">
+      <c r="N1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="O1" t="s" s="6">
+      <c r="O1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="P1" t="s" s="6">
+      <c r="P1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" t="s" s="6">
+      <c r="Q1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="R1" t="s" s="6">
+      <c r="R1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="S1" t="s" s="6">
+      <c r="S1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T1" t="s" s="6">
+      <c r="T1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="U1" t="s" s="6">
+      <c r="U1" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="7">
+    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s" s="7">
+      <c r="B2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s" s="6">
+      <c r="C2" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="D2" t="s" s="6">
-        <v>19</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
-      <c r="J2" t="s" s="6">
+      <c r="J2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K2" t="s" s="6">
+      <c r="L2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L2" t="s" s="6">
+      <c r="M2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="M2" t="s" s="6">
+      <c r="N2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N2" t="s" s="6">
+      <c r="O2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O2" t="s" s="6">
+      <c r="P2" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="P2" t="s" s="6">
-        <v>26</v>
       </c>
       <c r="Q2" s="9">
         <v>2018</v>
       </c>
-      <c r="R2" t="s" s="6">
+      <c r="R2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S2" t="s" s="6">
+      <c r="T2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T2" t="s" s="6">
+      <c r="U2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="U2" t="s" s="6">
+    </row>
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="6">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s" s="6">
+      <c r="C3" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="C3" t="s" s="6">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s" s="6">
-        <v>33</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
-      <c r="J3" t="s" s="6">
+      <c r="J3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K3" t="s" s="6">
-        <v>21</v>
-      </c>
       <c r="L3" s="8"/>
-      <c r="M3" t="s" s="6">
+      <c r="M3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N3" t="s" s="6">
+      <c r="O3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O3" t="s" s="6">
+      <c r="P3" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="P3" t="s" s="6">
-        <v>26</v>
       </c>
       <c r="Q3" s="9">
         <v>2018</v>
       </c>
-      <c r="R3" t="s" s="6">
+      <c r="R3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S3" t="s" s="6">
+      <c r="T3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T3" t="s" s="6">
+      <c r="U3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="U3" t="s" s="6">
-        <v>30</v>
-      </c>
     </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="6">
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s" s="6">
-        <v>34</v>
-      </c>
-      <c r="C4" t="s" s="6">
-        <v>35</v>
-      </c>
-      <c r="D4" t="s" s="6">
-        <v>36</v>
+      <c r="B4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
-      <c r="J4" t="s" s="6">
+      <c r="J4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K4" t="s" s="6">
-        <v>21</v>
-      </c>
       <c r="L4" s="8"/>
-      <c r="M4" t="s" s="6">
+      <c r="M4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N4" t="s" s="6">
+      <c r="O4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O4" t="s" s="6">
+      <c r="P4" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="P4" t="s" s="6">
-        <v>26</v>
       </c>
       <c r="Q4" s="9">
         <v>2018</v>
       </c>
-      <c r="R4" t="s" s="6">
+      <c r="R4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S4" t="s" s="6">
+      <c r="T4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T4" t="s" s="6">
+      <c r="U4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="U4" t="s" s="6">
-        <v>30</v>
-      </c>
     </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="6">
+    <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s" s="6">
+      <c r="B5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="C5" t="s" s="6">
-        <v>38</v>
-      </c>
-      <c r="D5" t="s" s="6">
-        <v>39</v>
-      </c>
-      <c r="E5" t="s" s="6">
-        <v>40</v>
-      </c>
-      <c r="F5" t="s" s="6">
-        <v>41</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
-      <c r="J5" t="s" s="6">
+      <c r="J5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K5" t="s" s="6">
-        <v>21</v>
-      </c>
       <c r="L5" s="8"/>
-      <c r="M5" t="s" s="6">
+      <c r="M5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N5" t="s" s="6">
+      <c r="O5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O5" t="s" s="6">
+      <c r="P5" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="P5" t="s" s="6">
-        <v>26</v>
       </c>
       <c r="Q5" s="9">
         <v>2018</v>
       </c>
-      <c r="R5" t="s" s="6">
+      <c r="R5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S5" t="s" s="6">
+      <c r="T5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T5" t="s" s="6">
+      <c r="U5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="U5" t="s" s="6">
-        <v>30</v>
-      </c>
     </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="6">
+    <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s" s="6">
-        <v>42</v>
-      </c>
-      <c r="C6" t="s" s="6">
-        <v>43</v>
-      </c>
-      <c r="D6" t="s" s="6">
-        <v>44</v>
+      <c r="B6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
-      <c r="J6" t="s" s="6">
+      <c r="J6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K6" t="s" s="6">
-        <v>21</v>
-      </c>
       <c r="L6" s="8"/>
-      <c r="M6" t="s" s="6">
+      <c r="M6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N6" t="s" s="6">
+      <c r="O6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O6" t="s" s="6">
+      <c r="P6" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="P6" t="s" s="6">
-        <v>26</v>
       </c>
       <c r="Q6" s="9">
         <v>2018</v>
       </c>
-      <c r="R6" t="s" s="6">
+      <c r="R6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S6" t="s" s="6">
+      <c r="T6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T6" t="s" s="6">
+      <c r="U6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="U6" t="s" s="6">
-        <v>30</v>
-      </c>
     </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="6">
+    <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s" s="6">
-        <v>45</v>
-      </c>
-      <c r="C7" t="s" s="6">
-        <v>46</v>
-      </c>
-      <c r="D7" t="s" s="6">
-        <v>47</v>
+      <c r="B7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
-      <c r="J7" t="s" s="6">
+      <c r="J7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K7" t="s" s="6">
-        <v>21</v>
-      </c>
       <c r="L7" s="8"/>
-      <c r="M7" t="s" s="6">
+      <c r="M7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N7" t="s" s="6">
+      <c r="O7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O7" t="s" s="6">
+      <c r="P7" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="P7" t="s" s="6">
-        <v>26</v>
       </c>
       <c r="Q7" s="9">
         <v>2018</v>
       </c>
-      <c r="R7" t="s" s="6">
+      <c r="R7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S7" t="s" s="6">
+      <c r="T7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T7" t="s" s="6">
+      <c r="U7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="U7" t="s" s="6">
-        <v>30</v>
-      </c>
     </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" t="s" s="6">
+    <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s" s="6">
-        <v>48</v>
-      </c>
-      <c r="C8" t="s" s="6">
-        <v>49</v>
-      </c>
-      <c r="D8" t="s" s="6">
-        <v>50</v>
+      <c r="B8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
-      <c r="J8" t="s" s="6">
+      <c r="J8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K8" t="s" s="6">
-        <v>21</v>
-      </c>
       <c r="L8" s="8"/>
-      <c r="M8" t="s" s="6">
+      <c r="M8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N8" t="s" s="6">
+      <c r="O8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O8" t="s" s="6">
+      <c r="P8" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="P8" t="s" s="6">
-        <v>26</v>
       </c>
       <c r="Q8" s="9">
         <v>2018</v>
       </c>
-      <c r="R8" t="s" s="6">
+      <c r="R8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S8" t="s" s="6">
+      <c r="T8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T8" t="s" s="6">
+      <c r="U8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="U8" t="s" s="6">
-        <v>30</v>
-      </c>
     </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" t="s" s="6">
+    <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s" s="6">
-        <v>51</v>
-      </c>
-      <c r="C9" t="s" s="6">
-        <v>52</v>
-      </c>
-      <c r="D9" t="s" s="6">
-        <v>53</v>
+      <c r="B9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
-      <c r="J9" t="s" s="6">
+      <c r="J9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K9" t="s" s="6">
-        <v>21</v>
-      </c>
       <c r="L9" s="8"/>
-      <c r="M9" t="s" s="6">
+      <c r="M9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N9" t="s" s="6">
+      <c r="O9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O9" t="s" s="6">
+      <c r="P9" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="P9" t="s" s="6">
-        <v>26</v>
       </c>
       <c r="Q9" s="9">
         <v>2018</v>
       </c>
-      <c r="R9" t="s" s="6">
+      <c r="R9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S9" t="s" s="6">
+      <c r="T9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T9" t="s" s="6">
+      <c r="U9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="U9" t="s" s="6">
-        <v>30</v>
-      </c>
     </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" t="s" s="6">
+    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s" s="6">
-        <v>54</v>
-      </c>
-      <c r="C10" t="s" s="6">
-        <v>55</v>
-      </c>
-      <c r="D10" t="s" s="6">
-        <v>56</v>
+      <c r="B10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
-      <c r="J10" t="s" s="6">
+      <c r="J10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K10" t="s" s="6">
-        <v>21</v>
-      </c>
       <c r="L10" s="8"/>
-      <c r="M10" t="s" s="6">
+      <c r="M10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N10" t="s" s="6">
+      <c r="O10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O10" t="s" s="6">
+      <c r="P10" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="P10" t="s" s="6">
-        <v>26</v>
       </c>
       <c r="Q10" s="9">
         <v>2018</v>
       </c>
-      <c r="R10" t="s" s="6">
+      <c r="R10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S10" t="s" s="6">
+      <c r="T10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T10" t="s" s="6">
+      <c r="U10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="U10" t="s" s="6">
-        <v>30</v>
-      </c>
     </row>
-    <row r="11" ht="15" customHeight="1">
-      <c r="A11" t="s" s="6">
+    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s" s="6">
-        <v>57</v>
-      </c>
-      <c r="C11" t="s" s="6">
-        <v>58</v>
-      </c>
-      <c r="D11" t="s" s="6">
-        <v>59</v>
+      <c r="B11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
-      <c r="J11" t="s" s="6">
+      <c r="J11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K11" t="s" s="6">
-        <v>21</v>
-      </c>
       <c r="L11" s="8"/>
-      <c r="M11" t="s" s="6">
+      <c r="M11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N11" t="s" s="6">
+      <c r="O11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O11" t="s" s="6">
+      <c r="P11" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="P11" t="s" s="6">
-        <v>26</v>
       </c>
       <c r="Q11" s="9">
         <v>2018</v>
       </c>
-      <c r="R11" t="s" s="6">
+      <c r="R11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S11" t="s" s="6">
+      <c r="T11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T11" t="s" s="6">
+      <c r="U11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="U11" t="s" s="6">
-        <v>30</v>
-      </c>
     </row>
-    <row r="12" ht="15" customHeight="1">
-      <c r="A12" t="s" s="6">
+    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B12" t="s" s="6">
-        <v>60</v>
-      </c>
-      <c r="C12" t="s" s="6">
-        <v>61</v>
-      </c>
-      <c r="D12" t="s" s="6">
-        <v>62</v>
+      <c r="B12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
-      <c r="J12" t="s" s="6">
+      <c r="J12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K12" t="s" s="6">
-        <v>21</v>
-      </c>
       <c r="L12" s="8"/>
-      <c r="M12" t="s" s="6">
+      <c r="M12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N12" t="s" s="6">
+      <c r="O12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O12" t="s" s="6">
+      <c r="P12" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="P12" t="s" s="6">
-        <v>26</v>
       </c>
       <c r="Q12" s="9">
         <v>2018</v>
       </c>
-      <c r="R12" t="s" s="6">
+      <c r="R12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S12" t="s" s="6">
+      <c r="T12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T12" t="s" s="6">
+      <c r="U12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="U12" t="s" s="6">
-        <v>30</v>
-      </c>
     </row>
-    <row r="13" ht="15" customHeight="1">
-      <c r="A13" t="s" s="6">
+    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B13" t="s" s="6">
-        <v>63</v>
-      </c>
-      <c r="C13" t="s" s="6">
-        <v>64</v>
-      </c>
-      <c r="D13" t="s" s="6">
-        <v>65</v>
-      </c>
-      <c r="E13" t="s" s="6">
-        <v>66</v>
-      </c>
-      <c r="F13" t="s" s="6">
-        <v>67</v>
+      <c r="B13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
-      <c r="J13" t="s" s="6">
+      <c r="J13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K13" t="s" s="6">
-        <v>21</v>
-      </c>
       <c r="L13" s="8"/>
-      <c r="M13" t="s" s="6">
+      <c r="M13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N13" t="s" s="6">
+      <c r="O13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O13" t="s" s="6">
+      <c r="P13" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="P13" t="s" s="6">
-        <v>26</v>
       </c>
       <c r="Q13" s="9">
         <v>2018</v>
       </c>
-      <c r="R13" t="s" s="6">
+      <c r="R13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S13" t="s" s="6">
+      <c r="T13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T13" t="s" s="6">
+      <c r="U13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="U13" t="s" s="6">
-        <v>30</v>
-      </c>
     </row>
-    <row r="14" ht="15" customHeight="1">
-      <c r="A14" t="s" s="6">
+    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B14" t="s" s="6">
-        <v>68</v>
-      </c>
-      <c r="C14" t="s" s="6">
-        <v>69</v>
-      </c>
-      <c r="D14" t="s" s="6">
-        <v>70</v>
-      </c>
-      <c r="E14" t="s" s="6">
-        <v>71</v>
+      <c r="B14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
-      <c r="J14" t="s" s="6">
+      <c r="J14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K14" t="s" s="6">
-        <v>21</v>
-      </c>
       <c r="L14" s="8"/>
-      <c r="M14" t="s" s="6">
+      <c r="M14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N14" t="s" s="6">
+      <c r="O14" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O14" t="s" s="6">
+      <c r="P14" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="P14" t="s" s="6">
-        <v>26</v>
       </c>
       <c r="Q14" s="9">
         <v>2018</v>
       </c>
-      <c r="R14" t="s" s="6">
+      <c r="R14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S14" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S14" t="s" s="6">
+      <c r="T14" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T14" t="s" s="6">
+      <c r="U14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="U14" t="s" s="6">
-        <v>30</v>
-      </c>
     </row>
-    <row r="15" ht="15" customHeight="1">
-      <c r="A15" t="s" s="6">
+    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B15" t="s" s="6">
-        <v>72</v>
-      </c>
-      <c r="C15" t="s" s="6">
-        <v>73</v>
-      </c>
-      <c r="D15" t="s" s="6">
-        <v>74</v>
+      <c r="B15" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
-      <c r="J15" t="s" s="6">
+      <c r="J15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K15" t="s" s="6">
-        <v>21</v>
-      </c>
       <c r="L15" s="8"/>
-      <c r="M15" t="s" s="6">
+      <c r="M15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N15" t="s" s="6">
+      <c r="O15" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O15" t="s" s="6">
+      <c r="P15" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="P15" t="s" s="6">
-        <v>26</v>
       </c>
       <c r="Q15" s="9">
         <v>2018</v>
       </c>
-      <c r="R15" t="s" s="6">
+      <c r="R15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S15" t="s" s="6">
+      <c r="T15" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T15" t="s" s="6">
+      <c r="U15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="U15" t="s" s="6">
-        <v>30</v>
-      </c>
     </row>
-    <row r="16" ht="15" customHeight="1">
-      <c r="A16" t="s" s="6">
+    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B16" t="s" s="6">
-        <v>75</v>
-      </c>
-      <c r="C16" t="s" s="6">
-        <v>76</v>
-      </c>
-      <c r="D16" t="s" s="6">
-        <v>77</v>
+      <c r="B16" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
-      <c r="J16" t="s" s="6">
+      <c r="J16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K16" t="s" s="6">
-        <v>21</v>
-      </c>
       <c r="L16" s="8"/>
-      <c r="M16" t="s" s="6">
+      <c r="M16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N16" t="s" s="6">
+      <c r="O16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O16" t="s" s="6">
+      <c r="P16" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="P16" t="s" s="6">
-        <v>26</v>
       </c>
       <c r="Q16" s="9">
         <v>2018</v>
       </c>
-      <c r="R16" t="s" s="6">
+      <c r="R16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S16" t="s" s="6">
+      <c r="T16" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T16" t="s" s="6">
+      <c r="U16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="U16" t="s" s="6">
-        <v>30</v>
-      </c>
     </row>
-    <row r="17" ht="15" customHeight="1">
-      <c r="A17" t="s" s="6">
+    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B17" t="s" s="6">
-        <v>78</v>
-      </c>
-      <c r="C17" t="s" s="6">
-        <v>79</v>
-      </c>
-      <c r="D17" t="s" s="6">
-        <v>80</v>
+      <c r="B17" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
-      <c r="J17" t="s" s="6">
+      <c r="J17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K17" t="s" s="6">
-        <v>21</v>
-      </c>
       <c r="L17" s="8"/>
-      <c r="M17" t="s" s="6">
+      <c r="M17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N17" t="s" s="6">
+      <c r="O17" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O17" t="s" s="6">
+      <c r="P17" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="P17" t="s" s="6">
-        <v>26</v>
       </c>
       <c r="Q17" s="9">
         <v>2018</v>
       </c>
-      <c r="R17" t="s" s="6">
+      <c r="R17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S17" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S17" t="s" s="6">
+      <c r="T17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T17" t="s" s="6">
+      <c r="U17" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="U17" t="s" s="6">
-        <v>30</v>
-      </c>
     </row>
-    <row r="18" ht="15" customHeight="1">
-      <c r="A18" t="s" s="6">
+    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B18" t="s" s="6">
-        <v>81</v>
-      </c>
-      <c r="C18" t="s" s="6">
-        <v>82</v>
-      </c>
-      <c r="D18" t="s" s="6">
-        <v>83</v>
+      <c r="B18" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
-      <c r="J18" t="s" s="6">
+      <c r="J18" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K18" t="s" s="6">
-        <v>21</v>
-      </c>
       <c r="L18" s="8"/>
-      <c r="M18" t="s" s="6">
+      <c r="M18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N18" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N18" t="s" s="6">
+      <c r="O18" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O18" t="s" s="6">
+      <c r="P18" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="P18" t="s" s="6">
-        <v>26</v>
       </c>
       <c r="Q18" s="9">
         <v>2018</v>
       </c>
-      <c r="R18" t="s" s="6">
+      <c r="R18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S18" t="s" s="6">
+      <c r="T18" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T18" t="s" s="6">
+      <c r="U18" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="U18" t="s" s="6">
-        <v>30</v>
-      </c>
     </row>
-    <row r="19" ht="15" customHeight="1">
-      <c r="A19" t="s" s="6">
+    <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B19" t="s" s="6">
-        <v>84</v>
-      </c>
-      <c r="C19" t="s" s="6">
-        <v>85</v>
-      </c>
-      <c r="D19" t="s" s="6">
-        <v>86</v>
+      <c r="B19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
-      <c r="J19" t="s" s="6">
+      <c r="J19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K19" t="s" s="6">
-        <v>21</v>
-      </c>
       <c r="L19" s="8"/>
-      <c r="M19" t="s" s="6">
+      <c r="M19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N19" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N19" t="s" s="6">
+      <c r="O19" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O19" t="s" s="6">
+      <c r="P19" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="P19" t="s" s="6">
-        <v>26</v>
       </c>
       <c r="Q19" s="9">
         <v>2018</v>
       </c>
-      <c r="R19" t="s" s="6">
+      <c r="R19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S19" t="s" s="6">
+      <c r="T19" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T19" t="s" s="6">
+      <c r="U19" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="U19" t="s" s="6">
-        <v>30</v>
-      </c>
     </row>
-    <row r="20" ht="15" customHeight="1">
-      <c r="A20" t="s" s="6">
+    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B20" t="s" s="6">
-        <v>87</v>
-      </c>
-      <c r="C20" t="s" s="6">
-        <v>88</v>
-      </c>
-      <c r="D20" t="s" s="6">
-        <v>89</v>
+      <c r="B20" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
-      <c r="J20" t="s" s="6">
+      <c r="J20" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K20" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K20" t="s" s="6">
-        <v>21</v>
-      </c>
       <c r="L20" s="8"/>
-      <c r="M20" t="s" s="6">
+      <c r="M20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N20" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N20" t="s" s="6">
+      <c r="O20" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O20" t="s" s="6">
+      <c r="P20" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="P20" t="s" s="6">
-        <v>26</v>
       </c>
       <c r="Q20" s="9">
         <v>2018</v>
       </c>
-      <c r="R20" t="s" s="6">
+      <c r="R20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S20" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S20" t="s" s="6">
+      <c r="T20" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T20" t="s" s="6">
+      <c r="U20" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="U20" t="s" s="6">
-        <v>30</v>
-      </c>
     </row>
-    <row r="21" ht="15" customHeight="1">
-      <c r="A21" t="s" s="6">
+    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B21" t="s" s="6">
-        <v>90</v>
-      </c>
-      <c r="C21" t="s" s="6">
-        <v>91</v>
-      </c>
-      <c r="D21" t="s" s="6">
-        <v>92</v>
+      <c r="B21" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
-      <c r="J21" t="s" s="6">
+      <c r="J21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K21" t="s" s="6">
-        <v>21</v>
-      </c>
       <c r="L21" s="8"/>
-      <c r="M21" t="s" s="6">
-        <v>93</v>
-      </c>
-      <c r="N21" t="s" s="6">
+      <c r="M21" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="O21" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O21" t="s" s="6">
+      <c r="P21" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="P21" t="s" s="6">
-        <v>26</v>
       </c>
       <c r="Q21" s="9">
         <v>2018</v>
       </c>
-      <c r="R21" t="s" s="6">
+      <c r="R21" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S21" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S21" t="s" s="6">
+      <c r="T21" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T21" t="s" s="6">
+      <c r="U21" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="U21" t="s" s="6">
-        <v>30</v>
-      </c>
     </row>
-    <row r="22" ht="15" customHeight="1">
-      <c r="A22" t="s" s="6">
+    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B22" t="s" s="6">
-        <v>94</v>
-      </c>
-      <c r="C22" t="s" s="6">
-        <v>95</v>
-      </c>
-      <c r="D22" t="s" s="6">
-        <v>96</v>
+      <c r="B22" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
-      <c r="J22" t="s" s="6">
+      <c r="J22" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K22" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K22" t="s" s="6">
-        <v>21</v>
-      </c>
       <c r="L22" s="8"/>
-      <c r="M22" t="s" s="6">
+      <c r="M22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N22" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N22" t="s" s="6">
+      <c r="O22" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O22" t="s" s="6">
+      <c r="P22" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="P22" t="s" s="6">
-        <v>26</v>
       </c>
       <c r="Q22" s="9">
         <v>2018</v>
       </c>
-      <c r="R22" t="s" s="6">
+      <c r="R22" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S22" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S22" t="s" s="6">
+      <c r="T22" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T22" t="s" s="6">
+      <c r="U22" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="U22" t="s" s="6">
-        <v>30</v>
-      </c>
     </row>
-    <row r="23" ht="15" customHeight="1">
-      <c r="A23" t="s" s="6">
+    <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B23" t="s" s="6">
-        <v>97</v>
-      </c>
-      <c r="C23" t="s" s="6">
-        <v>98</v>
-      </c>
-      <c r="D23" t="s" s="6">
-        <v>99</v>
+      <c r="B23" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
-      <c r="J23" t="s" s="6">
+      <c r="J23" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K23" t="s" s="6">
-        <v>21</v>
-      </c>
       <c r="L23" s="8"/>
-      <c r="M23" t="s" s="6">
+      <c r="M23" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N23" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N23" t="s" s="6">
+      <c r="O23" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O23" t="s" s="6">
+      <c r="P23" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="P23" t="s" s="6">
-        <v>26</v>
       </c>
       <c r="Q23" s="9">
         <v>2018</v>
       </c>
-      <c r="R23" t="s" s="6">
+      <c r="R23" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S23" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S23" t="s" s="6">
+      <c r="T23" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T23" t="s" s="6">
+      <c r="U23" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="U23" t="s" s="6">
-        <v>30</v>
-      </c>
     </row>
-    <row r="24" ht="15" customHeight="1">
-      <c r="A24" t="s" s="6">
+    <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B24" t="s" s="6">
-        <v>100</v>
-      </c>
-      <c r="C24" t="s" s="6">
-        <v>101</v>
-      </c>
-      <c r="D24" t="s" s="6">
-        <v>102</v>
+      <c r="B24" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
-      <c r="J24" t="s" s="6">
+      <c r="J24" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K24" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K24" t="s" s="6">
-        <v>21</v>
-      </c>
       <c r="L24" s="8"/>
-      <c r="M24" t="s" s="6">
+      <c r="M24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N24" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N24" t="s" s="6">
+      <c r="O24" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O24" t="s" s="6">
+      <c r="P24" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="P24" t="s" s="6">
-        <v>26</v>
       </c>
       <c r="Q24" s="9">
         <v>2018</v>
       </c>
-      <c r="R24" t="s" s="6">
+      <c r="R24" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S24" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S24" t="s" s="6">
+      <c r="T24" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T24" t="s" s="6">
+      <c r="U24" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="U24" t="s" s="6">
-        <v>30</v>
-      </c>
     </row>
-    <row r="25" ht="15" customHeight="1">
-      <c r="A25" t="s" s="6">
+    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B25" t="s" s="6">
-        <v>103</v>
-      </c>
-      <c r="C25" t="s" s="6">
-        <v>104</v>
-      </c>
-      <c r="D25" t="s" s="6">
-        <v>105</v>
+      <c r="B25" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
-      <c r="J25" t="s" s="6">
+      <c r="J25" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K25" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K25" t="s" s="6">
-        <v>21</v>
-      </c>
       <c r="L25" s="8"/>
-      <c r="M25" t="s" s="6">
+      <c r="M25" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N25" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N25" t="s" s="6">
+      <c r="O25" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O25" t="s" s="6">
+      <c r="P25" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="P25" t="s" s="6">
-        <v>26</v>
       </c>
       <c r="Q25" s="9">
         <v>2018</v>
       </c>
-      <c r="R25" t="s" s="6">
+      <c r="R25" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S25" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S25" t="s" s="6">
+      <c r="T25" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T25" t="s" s="6">
+      <c r="U25" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="U25" t="s" s="6">
-        <v>30</v>
-      </c>
     </row>
-    <row r="26" ht="15" customHeight="1">
-      <c r="A26" t="s" s="6">
+    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B26" t="s" s="6">
-        <v>106</v>
-      </c>
-      <c r="C26" t="s" s="6">
-        <v>107</v>
-      </c>
-      <c r="D26" t="s" s="6">
+      <c r="B26" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>108</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>83</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
-      <c r="J26" t="s" s="6">
+      <c r="J26" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K26" t="s" s="6">
-        <v>21</v>
-      </c>
       <c r="L26" s="8"/>
-      <c r="M26" t="s" s="6">
+      <c r="M26" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N26" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N26" t="s" s="6">
+      <c r="O26" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O26" t="s" s="6">
+      <c r="P26" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="P26" t="s" s="6">
-        <v>26</v>
       </c>
       <c r="Q26" s="9">
         <v>2018</v>
       </c>
-      <c r="R26" t="s" s="6">
+      <c r="R26" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S26" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S26" t="s" s="6">
+      <c r="T26" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T26" t="s" s="6">
+      <c r="U26" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="U26" t="s" s="6">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>